<commit_message>
Update thesis and excel
</commit_message>
<xml_diff>
--- a/static/thesis_template.xlsx
+++ b/static/thesis_template.xlsx
@@ -1,99 +1,177 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5D2EBC-6992-4138-A3DE-69CEF1F68FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D95CE55-5834-4B05-A79D-39222784EF74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="File mẫu" sheetId="1" r:id="rId1"/>
+    <sheet name="Chuyên ngành" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>TRƯỜNG ĐẠI HỌC CÔNG THƯƠNG</t>
+  </si>
+  <si>
+    <t>THÀNH PHỐ HỒ CHÍ MINH</t>
+  </si>
+  <si>
+    <t>KHOA CÔNG NGHỆ THÔNG TIN</t>
+  </si>
+  <si>
+    <t>DANH SÁCH ĐỀ TÀI ĐỒ ÁN CHUYÊN NGÀNH CỦA SINH VIÊN KHÓA 12 NGÀNH CNTT</t>
+  </si>
   <si>
     <t>STT</t>
   </si>
   <si>
-    <t>TÊN ĐỀ TÀI</t>
-  </si>
-  <si>
-    <t>NỘI DUNG YÊU CẦU</t>
-  </si>
-  <si>
-    <t>GIÁO VIÊN HƯỚNG DẪN</t>
-  </si>
-  <si>
-    <t>EMAIL</t>
-  </si>
-  <si>
-    <t>BỘ MÔN</t>
+    <t>TÊN ĐỀ TÀI *</t>
+  </si>
+  <si>
+    <t>NỘI DUNG YÊU CẦU *</t>
+  </si>
+  <si>
+    <t>MÃ GV HƯỚNG DẪN *</t>
+  </si>
+  <si>
+    <t>LOẠI ĐỀ TÀI *
+1: Khóa luận kỹ sư
+2: Đồ án tốt nghiệp</t>
+  </si>
+  <si>
+    <t>MÃ GV PHẢN BIỆN
+(Nếu loại đề tài là 2 thì có thể nhập MÃ GV PHẢN BIỆN hoặc không)</t>
+  </si>
+  <si>
+    <t>BỘ MÔN *
+1: KTPM
+2: HTTT
+3: KHDL&amp;TTNT
+4: MMT-ATTT</t>
   </si>
   <si>
     <t>GHI CHÚ</t>
   </si>
   <si>
-    <t>MÃ GIẢNG VIÊN</t>
-  </si>
-  <si>
-    <t>TRƯỜNG ĐẠI HỌC CÔNG THƯƠNG</t>
-  </si>
-  <si>
-    <t>THÀNH PHỐ HỒ CHÍ MINH</t>
-  </si>
-  <si>
-    <t>KHOA CÔNG NGHỆ THÔNG TIN</t>
-  </si>
-  <si>
-    <t>DANH SÁCH ĐỀ TÀI ĐỒ ÁN CHUYÊN NGÀNH CỦA SINH VIÊN KHÓA 12 NGÀNH CNTT</t>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>4c5ccb13-e1da-48de-a067-a7fdd547040c</t>
+  </si>
+  <si>
+    <t>Công nghệ thông tin</t>
+  </si>
+  <si>
+    <t>57c895c3-f687-49da-9891-6f2bb98b8a9b</t>
+  </si>
+  <si>
+    <t>An toàn thông tin</t>
+  </si>
+  <si>
+    <t>CHUYÊN NGÀNH *
+(Chọn chuyên ngành bằng dropdown)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
     </font>
   </fonts>
   <fills count="2">
@@ -131,22 +209,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -163,6 +256,13 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/customStorage/customStorage.xml><?xml version="1.0" encoding="utf-8"?>
+<customStorage xmlns="https://web.wps.cn/et/2018/main">
+  <book/>
+  <sheets/>
+</customStorage>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -452,96 +552,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="60.77734375" customWidth="1"/>
-    <col min="4" max="4" width="28.77734375" customWidth="1"/>
-    <col min="5" max="5" width="24.5546875" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
-    <col min="7" max="7" width="21.44140625" customWidth="1"/>
-    <col min="8" max="8" width="19.88671875" customWidth="1"/>
-    <col min="9" max="9" width="33.33203125" customWidth="1"/>
-    <col min="10" max="10" width="78.109375" customWidth="1"/>
+    <col min="4" max="4" width="38.21875" customWidth="1"/>
+    <col min="5" max="5" width="28.77734375" customWidth="1"/>
+    <col min="6" max="6" width="24.5546875" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" customWidth="1"/>
+    <col min="8" max="9" width="21.44140625" customWidth="1"/>
+    <col min="10" max="10" width="19.88671875" customWidth="1"/>
+    <col min="11" max="11" width="33.33203125" customWidth="1"/>
+    <col min="12" max="12" width="78.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12" ht="24" customHeight="1">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="E1" s="1"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+    </row>
+    <row r="2" spans="1:12" ht="18" customHeight="1">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" ht="24.6" customHeight="1">
+      <c r="A3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" ht="40.200000000000003" customHeight="1">
+      <c r="A4" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+    </row>
+    <row r="5" spans="1:12" ht="72">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="F5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:10" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="G5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:10" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="H5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" ht="19.05" customHeight="1">
       <c r="A6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="23.4" customHeight="1">
       <c r="A7">
         <v>2</v>
       </c>
@@ -551,8 +657,63 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{294B46FF-9CBF-426C-9420-AF36FB39FBE0}">
+          <x14:formula1>
+            <xm:f>'Chuyên ngành'!$B$2:$B$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>H6:H300</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="43.44140625" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>